<commit_message>
fixed the error, which occured in the demo
</commit_message>
<xml_diff>
--- a/roundtable.xlsx
+++ b/roundtable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="122">
   <si>
     <t>Synergy Roundtable</t>
   </si>
@@ -226,6 +226,147 @@
     <t>10:00:42:db:36:d0:00:67</t>
   </si>
   <si>
+    <t>CTC Synergy HE11, bay 2</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:90</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:91</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:98</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:99</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 2</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:32:50</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:91</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:32:58</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:93</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 6</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:10</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:11</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:18</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:19</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 1</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:70</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:8d</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:78</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:8f</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 3</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:4B:A0</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:4B:A1</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:4B:A8</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:4B:A9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:50</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:c9</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:58</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:cb</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 6</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen9</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C0</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C1</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C8</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 4</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:20</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:45:21</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:28</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:45:29</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 5</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:10</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:11</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:18</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:19</t>
+  </si>
+  <si>
     <t>CTC Synergy HE01, bay 9</t>
   </si>
   <si>
@@ -239,150 +380,6 @@
   </si>
   <si>
     <t>10:00:94:F1:28:96:65:89</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 2</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:90</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:91</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:98</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:99</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 2</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:50</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:91</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:58</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:93</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 6</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:10</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:11</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:18</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 5</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:10</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:11</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:18</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 1</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:70</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8d</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:78</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8f</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 3</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:4B:A0</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:4B:A1</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:4B:A8</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:4B:A9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:50</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:c9</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:58</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:cb</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 6</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen9</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C0</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C1</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C8</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 4</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:20</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:01:21</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:28</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:01:23</t>
   </si>
 </sst>
 </file>
@@ -2463,10 +2460,10 @@
         <v>70</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C102">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D102" t="s">
         <v>71</v>
@@ -2480,10 +2477,10 @@
         <v>70</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C103">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D103" t="s">
         <v>71</v>
@@ -2500,10 +2497,10 @@
         <v>70</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C104">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D104" t="s">
         <v>71</v>
@@ -2517,10 +2514,10 @@
         <v>70</v>
       </c>
       <c r="B105" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C105">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D105" t="s">
         <v>71</v>
@@ -2534,10 +2531,10 @@
         <v>70</v>
       </c>
       <c r="B106" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C106">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D106" t="s">
         <v>73</v>
@@ -2551,10 +2548,10 @@
         <v>70</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C107">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D107" t="s">
         <v>73</v>
@@ -2571,10 +2568,10 @@
         <v>70</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C108">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D108" t="s">
         <v>73</v>
@@ -2588,10 +2585,10 @@
         <v>70</v>
       </c>
       <c r="B109" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C109">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D109" t="s">
         <v>73</v>
@@ -2608,7 +2605,7 @@
         <v>35</v>
       </c>
       <c r="C110">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D110" t="s">
         <v>76</v>
@@ -2625,7 +2622,7 @@
         <v>35</v>
       </c>
       <c r="C111">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D111" t="s">
         <v>76</v>
@@ -2645,7 +2642,7 @@
         <v>35</v>
       </c>
       <c r="C112">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D112" t="s">
         <v>76</v>
@@ -2662,7 +2659,7 @@
         <v>35</v>
       </c>
       <c r="C113">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D113" t="s">
         <v>76</v>
@@ -2679,7 +2676,7 @@
         <v>35</v>
       </c>
       <c r="C114">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D114" t="s">
         <v>78</v>
@@ -2696,7 +2693,7 @@
         <v>35</v>
       </c>
       <c r="C115">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D115" t="s">
         <v>78</v>
@@ -2716,7 +2713,7 @@
         <v>35</v>
       </c>
       <c r="C116">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D116" t="s">
         <v>78</v>
@@ -2733,7 +2730,7 @@
         <v>35</v>
       </c>
       <c r="C117">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D117" t="s">
         <v>78</v>
@@ -2750,7 +2747,7 @@
         <v>35</v>
       </c>
       <c r="C118">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D118" t="s">
         <v>81</v>
@@ -2767,7 +2764,7 @@
         <v>35</v>
       </c>
       <c r="C119">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D119" t="s">
         <v>81</v>
@@ -2787,7 +2784,7 @@
         <v>35</v>
       </c>
       <c r="C120">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D120" t="s">
         <v>81</v>
@@ -2804,7 +2801,7 @@
         <v>35</v>
       </c>
       <c r="C121">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D121" t="s">
         <v>81</v>
@@ -2821,7 +2818,7 @@
         <v>35</v>
       </c>
       <c r="C122">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D122" t="s">
         <v>83</v>
@@ -2838,7 +2835,7 @@
         <v>35</v>
       </c>
       <c r="C123">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D123" t="s">
         <v>83</v>
@@ -2858,7 +2855,7 @@
         <v>35</v>
       </c>
       <c r="C124">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D124" t="s">
         <v>83</v>
@@ -2875,7 +2872,7 @@
         <v>35</v>
       </c>
       <c r="C125">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D125" t="s">
         <v>83</v>
@@ -2892,7 +2889,7 @@
         <v>35</v>
       </c>
       <c r="C126">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D126" t="s">
         <v>86</v>
@@ -2909,7 +2906,7 @@
         <v>35</v>
       </c>
       <c r="C127">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D127" t="s">
         <v>86</v>
@@ -2929,7 +2926,7 @@
         <v>35</v>
       </c>
       <c r="C128">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D128" t="s">
         <v>86</v>
@@ -2946,7 +2943,7 @@
         <v>35</v>
       </c>
       <c r="C129">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D129" t="s">
         <v>86</v>
@@ -2963,7 +2960,7 @@
         <v>35</v>
       </c>
       <c r="C130">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D130" t="s">
         <v>88</v>
@@ -2980,7 +2977,7 @@
         <v>35</v>
       </c>
       <c r="C131">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D131" t="s">
         <v>88</v>
@@ -3000,7 +2997,7 @@
         <v>35</v>
       </c>
       <c r="C132">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D132" t="s">
         <v>88</v>
@@ -3017,7 +3014,7 @@
         <v>35</v>
       </c>
       <c r="C133">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D133" t="s">
         <v>88</v>
@@ -3031,13 +3028,13 @@
         <v>90</v>
       </c>
       <c r="B134" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C134">
         <v>32768</v>
       </c>
       <c r="D134" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -3048,16 +3045,16 @@
         <v>90</v>
       </c>
       <c r="B135" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C135">
         <v>32768</v>
       </c>
       <c r="D135" t="s">
+        <v>91</v>
+      </c>
+      <c r="E135" t="s">
         <v>92</v>
-      </c>
-      <c r="E135" t="s">
-        <v>93</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -3068,13 +3065,13 @@
         <v>90</v>
       </c>
       <c r="B136" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C136">
         <v>32768</v>
       </c>
       <c r="D136" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F136" t="s">
         <v>10</v>
@@ -3085,13 +3082,13 @@
         <v>90</v>
       </c>
       <c r="B137" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C137">
         <v>32768</v>
       </c>
       <c r="D137" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F137" t="s">
         <v>10</v>
@@ -3102,13 +3099,13 @@
         <v>90</v>
       </c>
       <c r="B138" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C138">
         <v>32768</v>
       </c>
       <c r="D138" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F138" t="s">
         <v>10</v>
@@ -3119,16 +3116,16 @@
         <v>90</v>
       </c>
       <c r="B139" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C139">
         <v>32768</v>
       </c>
       <c r="D139" t="s">
+        <v>93</v>
+      </c>
+      <c r="E139" t="s">
         <v>94</v>
-      </c>
-      <c r="E139" t="s">
-        <v>95</v>
       </c>
       <c r="F139" t="s">
         <v>10</v>
@@ -3139,13 +3136,13 @@
         <v>90</v>
       </c>
       <c r="B140" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C140">
         <v>32768</v>
       </c>
       <c r="D140" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F140" t="s">
         <v>10</v>
@@ -3156,13 +3153,13 @@
         <v>90</v>
       </c>
       <c r="B141" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C141">
         <v>32768</v>
       </c>
       <c r="D141" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F141" t="s">
         <v>10</v>
@@ -3170,16 +3167,16 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
+        <v>95</v>
+      </c>
+      <c r="B142" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142">
+        <v>262144</v>
+      </c>
+      <c r="D142" t="s">
         <v>96</v>
-      </c>
-      <c r="B142" t="s">
-        <v>35</v>
-      </c>
-      <c r="C142">
-        <v>65536</v>
-      </c>
-      <c r="D142" t="s">
-        <v>97</v>
       </c>
       <c r="F142" t="s">
         <v>10</v>
@@ -3187,19 +3184,19 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
+        <v>95</v>
+      </c>
+      <c r="B143" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143">
+        <v>262144</v>
+      </c>
+      <c r="D143" t="s">
         <v>96</v>
       </c>
-      <c r="B143" t="s">
-        <v>35</v>
-      </c>
-      <c r="C143">
-        <v>65536</v>
-      </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>97</v>
-      </c>
-      <c r="E143" t="s">
-        <v>98</v>
       </c>
       <c r="F143" t="s">
         <v>10</v>
@@ -3207,16 +3204,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
+        <v>95</v>
+      </c>
+      <c r="B144" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144">
+        <v>262144</v>
+      </c>
+      <c r="D144" t="s">
         <v>96</v>
-      </c>
-      <c r="B144" t="s">
-        <v>35</v>
-      </c>
-      <c r="C144">
-        <v>65536</v>
-      </c>
-      <c r="D144" t="s">
-        <v>97</v>
       </c>
       <c r="F144" t="s">
         <v>10</v>
@@ -3224,16 +3221,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
+        <v>95</v>
+      </c>
+      <c r="B145" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145">
+        <v>262144</v>
+      </c>
+      <c r="D145" t="s">
         <v>96</v>
-      </c>
-      <c r="B145" t="s">
-        <v>35</v>
-      </c>
-      <c r="C145">
-        <v>65536</v>
-      </c>
-      <c r="D145" t="s">
-        <v>97</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
@@ -3241,16 +3238,16 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B146" t="s">
         <v>35</v>
       </c>
       <c r="C146">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D146" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -3258,19 +3255,19 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B147" t="s">
         <v>35</v>
       </c>
       <c r="C147">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D147" t="s">
+        <v>98</v>
+      </c>
+      <c r="E147" t="s">
         <v>99</v>
-      </c>
-      <c r="E147" t="s">
-        <v>100</v>
       </c>
       <c r="F147" t="s">
         <v>10</v>
@@ -3278,16 +3275,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B148" t="s">
         <v>35</v>
       </c>
       <c r="C148">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D148" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F148" t="s">
         <v>10</v>
@@ -3295,16 +3292,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B149" t="s">
         <v>35</v>
       </c>
       <c r="C149">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D149" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F149" t="s">
         <v>10</v>
@@ -3312,13 +3309,13 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
+        <v>100</v>
+      </c>
+      <c r="B150" t="s">
         <v>101</v>
       </c>
-      <c r="B150" t="s">
-        <v>8</v>
-      </c>
       <c r="C150">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D150" t="s">
         <v>102</v>
@@ -3329,13 +3326,13 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
+        <v>100</v>
+      </c>
+      <c r="B151" t="s">
         <v>101</v>
       </c>
-      <c r="B151" t="s">
-        <v>8</v>
-      </c>
       <c r="C151">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D151" t="s">
         <v>102</v>
@@ -3349,13 +3346,13 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
+        <v>100</v>
+      </c>
+      <c r="B152" t="s">
         <v>101</v>
       </c>
-      <c r="B152" t="s">
-        <v>8</v>
-      </c>
       <c r="C152">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D152" t="s">
         <v>102</v>
@@ -3366,13 +3363,13 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
+        <v>100</v>
+      </c>
+      <c r="B153" t="s">
         <v>101</v>
       </c>
-      <c r="B153" t="s">
-        <v>8</v>
-      </c>
       <c r="C153">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D153" t="s">
         <v>102</v>
@@ -3383,13 +3380,13 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
+        <v>100</v>
+      </c>
+      <c r="B154" t="s">
         <v>101</v>
       </c>
-      <c r="B154" t="s">
-        <v>8</v>
-      </c>
       <c r="C154">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D154" t="s">
         <v>104</v>
@@ -3400,13 +3397,13 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
+        <v>100</v>
+      </c>
+      <c r="B155" t="s">
         <v>101</v>
       </c>
-      <c r="B155" t="s">
-        <v>8</v>
-      </c>
       <c r="C155">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D155" t="s">
         <v>104</v>
@@ -3420,13 +3417,13 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
+        <v>100</v>
+      </c>
+      <c r="B156" t="s">
         <v>101</v>
       </c>
-      <c r="B156" t="s">
-        <v>8</v>
-      </c>
       <c r="C156">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D156" t="s">
         <v>104</v>
@@ -3437,13 +3434,13 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
+        <v>100</v>
+      </c>
+      <c r="B157" t="s">
         <v>101</v>
       </c>
-      <c r="B157" t="s">
-        <v>8</v>
-      </c>
       <c r="C157">
-        <v>32768</v>
+        <v>131072</v>
       </c>
       <c r="D157" t="s">
         <v>104</v>
@@ -3457,10 +3454,10 @@
         <v>106</v>
       </c>
       <c r="B158" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C158">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D158" t="s">
         <v>107</v>
@@ -3474,10 +3471,10 @@
         <v>106</v>
       </c>
       <c r="B159" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C159">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D159" t="s">
         <v>107</v>
@@ -3494,10 +3491,10 @@
         <v>106</v>
       </c>
       <c r="B160" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C160">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D160" t="s">
         <v>107</v>
@@ -3511,10 +3508,10 @@
         <v>106</v>
       </c>
       <c r="B161" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C161">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D161" t="s">
         <v>107</v>
@@ -3528,10 +3525,10 @@
         <v>106</v>
       </c>
       <c r="B162" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C162">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D162" t="s">
         <v>109</v>
@@ -3545,10 +3542,10 @@
         <v>106</v>
       </c>
       <c r="B163" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C163">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D163" t="s">
         <v>109</v>
@@ -3565,10 +3562,10 @@
         <v>106</v>
       </c>
       <c r="B164" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C164">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D164" t="s">
         <v>109</v>
@@ -3582,10 +3579,10 @@
         <v>106</v>
       </c>
       <c r="B165" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C165">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D165" t="s">
         <v>109</v>
@@ -3602,13 +3599,13 @@
         <v>112</v>
       </c>
       <c r="C166">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D166" t="s">
         <v>113</v>
       </c>
       <c r="F166" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -3619,16 +3616,16 @@
         <v>112</v>
       </c>
       <c r="C167">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D167" t="s">
         <v>113</v>
       </c>
       <c r="E167" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F167" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -3639,13 +3636,13 @@
         <v>112</v>
       </c>
       <c r="C168">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D168" t="s">
         <v>113</v>
       </c>
       <c r="F168" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -3656,13 +3653,13 @@
         <v>112</v>
       </c>
       <c r="C169">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D169" t="s">
         <v>113</v>
       </c>
       <c r="F169" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -3673,13 +3670,13 @@
         <v>112</v>
       </c>
       <c r="C170">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D170" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F170" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -3690,16 +3687,16 @@
         <v>112</v>
       </c>
       <c r="C171">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D171" t="s">
+        <v>115</v>
+      </c>
+      <c r="E171" t="s">
         <v>116</v>
       </c>
-      <c r="E171" t="s">
-        <v>117</v>
-      </c>
       <c r="F171" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -3710,13 +3707,13 @@
         <v>112</v>
       </c>
       <c r="C172">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D172" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F172" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -3727,27 +3724,27 @@
         <v>112</v>
       </c>
       <c r="C173">
-        <v>131072</v>
+        <v>32768</v>
       </c>
       <c r="D173" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F173" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
+        <v>117</v>
+      </c>
+      <c r="B174" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>16384</v>
+      </c>
+      <c r="D174" t="s">
         <v>118</v>
-      </c>
-      <c r="B174" t="s">
-        <v>8</v>
-      </c>
-      <c r="C174">
-        <v>65536</v>
-      </c>
-      <c r="D174" t="s">
-        <v>119</v>
       </c>
       <c r="F174" t="s">
         <v>10</v>
@@ -3755,19 +3752,19 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
+        <v>117</v>
+      </c>
+      <c r="B175" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>16384</v>
+      </c>
+      <c r="D175" t="s">
         <v>118</v>
       </c>
-      <c r="B175" t="s">
-        <v>8</v>
-      </c>
-      <c r="C175">
-        <v>65536</v>
-      </c>
-      <c r="D175" t="s">
+      <c r="E175" t="s">
         <v>119</v>
-      </c>
-      <c r="E175" t="s">
-        <v>120</v>
       </c>
       <c r="F175" t="s">
         <v>10</v>
@@ -3775,16 +3772,16 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" t="s">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <v>16384</v>
+      </c>
+      <c r="D176" t="s">
         <v>118</v>
-      </c>
-      <c r="B176" t="s">
-        <v>8</v>
-      </c>
-      <c r="C176">
-        <v>65536</v>
-      </c>
-      <c r="D176" t="s">
-        <v>119</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -3792,16 +3789,16 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
+        <v>117</v>
+      </c>
+      <c r="B177" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177">
+        <v>16384</v>
+      </c>
+      <c r="D177" t="s">
         <v>118</v>
-      </c>
-      <c r="B177" t="s">
-        <v>8</v>
-      </c>
-      <c r="C177">
-        <v>65536</v>
-      </c>
-      <c r="D177" t="s">
-        <v>119</v>
       </c>
       <c r="F177" t="s">
         <v>10</v>
@@ -3809,16 +3806,16 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
       </c>
       <c r="C178">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D178" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
@@ -3826,19 +3823,19 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B179" t="s">
         <v>8</v>
       </c>
       <c r="C179">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D179" t="s">
+        <v>120</v>
+      </c>
+      <c r="E179" t="s">
         <v>121</v>
-      </c>
-      <c r="E179" t="s">
-        <v>122</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -3846,16 +3843,16 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B180" t="s">
         <v>8</v>
       </c>
       <c r="C180">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D180" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F180" t="s">
         <v>10</v>
@@ -3863,16 +3860,16 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B181" t="s">
         <v>8</v>
       </c>
       <c r="C181">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D181" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
new changes, as we rebuild our Synergy Landscape
</commit_message>
<xml_diff>
--- a/roundtable.xlsx
+++ b/roundtable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="123">
   <si>
     <t>Synergy Roundtable</t>
   </si>
@@ -64,6 +64,9 @@
     <t>9C:DC:71:E1:63:70</t>
   </si>
   <si>
+    <t>Warning</t>
+  </si>
+  <si>
     <t>10:00:9C:DC:71:E1:63:71</t>
   </si>
   <si>
@@ -73,6 +76,225 @@
     <t>10:00:9C:DC:71:E1:63:79</t>
   </si>
   <si>
+    <t>CTC Synergy HE11, bay 5</t>
+  </si>
+  <si>
+    <t>Synergy 480 Gen9</t>
+  </si>
+  <si>
+    <t>94:18:82:39:21:F0</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:21:F1</t>
+  </si>
+  <si>
+    <t>94:18:82:39:21:F8</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:21:F9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:70</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:04:71</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:78</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:04:79</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 9</t>
+  </si>
+  <si>
+    <t>94:18:82:39:9B:60</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:9B:61</t>
+  </si>
+  <si>
+    <t>94:18:82:39:9B:68</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:9B:69</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 2</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:90</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:91</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:98</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:99</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 2</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:32:50</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:91</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:32:58</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:93</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 6</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:10</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:11</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:18</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:19</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 1</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:70</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:8d</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:78</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:00:8f</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:50</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:02:0b</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:58</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:02:0d</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 3</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:4B:A0</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:01:d1</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:4B:A8</t>
+  </si>
+  <si>
+    <t>10:00:42:db:36:d0:01:d3</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 5</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:10</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:11</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:18</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:19</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 4</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:20</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:45:21</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:28</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:45:29</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 6</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen9</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C0</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C1</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C8</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 8</t>
+  </si>
+  <si>
+    <t>94:18:82:39:68:20</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:68:21</t>
+  </si>
+  <si>
+    <t>94:18:82:39:68:28</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:68:29</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 7</t>
+  </si>
+  <si>
+    <t>94:18:82:39:E3:E0</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:E3:E1</t>
+  </si>
+  <si>
+    <t>94:18:82:39:E3:E8</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:E3:E9</t>
+  </si>
+  <si>
     <t>CTC Synergy HE01, bay 2</t>
   </si>
   <si>
@@ -88,42 +310,69 @@
     <t>10:00:9C:DC:71:E1:5B:09</t>
   </si>
   <si>
+    <t>CTC Synergy HE01, bay 3</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:99:00</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:E1:99:01</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:99:08</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:E1:99:09</t>
+  </si>
+  <si>
     <t>CTC Synergy HE01, bay 8</t>
   </si>
   <si>
     <t>94:F1:28:96:63:A0</t>
   </si>
   <si>
-    <t>10:00:94:F1:28:96:63:A1</t>
+    <t>10:00:42:db:36:d0:01:c5</t>
   </si>
   <si>
     <t>94:F1:28:96:63:A8</t>
   </si>
   <si>
-    <t>10:00:94:F1:28:96:63:A9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 3</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:99:00</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:99:01</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:99:08</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:99:09</t>
+    <t>10:00:42:db:36:d0:01:c7</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 9</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:65:80</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:65:81</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:65:88</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:65:89</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 4</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:60</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:61</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:68</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:69</t>
   </si>
   <si>
     <t>CTC Synergy HE11, bay 3</t>
   </si>
   <si>
-    <t>Synergy 480 Gen9</t>
-  </si>
-  <si>
     <t>9C:DC:71:9D:00:50</t>
   </si>
   <si>
@@ -134,252 +383,6 @@
   </si>
   <si>
     <t>10:00:9C:DC:71:9D:00:59</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 7</t>
-  </si>
-  <si>
-    <t>94:18:82:39:E3:E0</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:E3:E1</t>
-  </si>
-  <si>
-    <t>94:18:82:39:E3:E8</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:E3:E9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 5</t>
-  </si>
-  <si>
-    <t>94:18:82:39:21:F0</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:21:F1</t>
-  </si>
-  <si>
-    <t>94:18:82:39:21:F8</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:21:F9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 8</t>
-  </si>
-  <si>
-    <t>94:18:82:39:68:20</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:68:21</t>
-  </si>
-  <si>
-    <t>94:18:82:39:68:28</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:68:29</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 4</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:60</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:61</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:68</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:69</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:70</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:04:71</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:78</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:04:79</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 9</t>
-  </si>
-  <si>
-    <t>94:18:82:39:9B:60</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:65</t>
-  </si>
-  <si>
-    <t>94:18:82:39:9B:68</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:67</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 2</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:90</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:91</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:98</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:99</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 2</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:50</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:91</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:58</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:93</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 6</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:10</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:11</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:18</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 1</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:70</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8d</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:78</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8f</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 3</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:4B:A0</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:4B:A1</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:4B:A8</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:4B:A9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:50</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:c9</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:58</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:cb</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 6</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen9</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C0</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C1</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C8</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 4</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:20</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:45:21</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:28</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:45:29</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 5</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:10</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:11</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:18</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 9</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:65:80</t>
-  </si>
-  <si>
-    <t>10:00:94:F1:28:96:65:81</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:65:88</t>
-  </si>
-  <si>
-    <t>10:00:94:F1:28:96:65:89</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -924,10 +927,10 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
         <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -944,7 +947,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -961,7 +964,7 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -975,10 +978,10 @@
         <v>16384</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -992,13 +995,13 @@
         <v>16384</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1012,10 +1015,10 @@
         <v>16384</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1029,24 +1032,24 @@
         <v>16384</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C22">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
@@ -1054,19 +1057,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -1074,16 +1077,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
@@ -1091,16 +1094,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
@@ -1108,16 +1111,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C26">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -1125,19 +1128,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C27">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -1145,16 +1148,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
@@ -1162,16 +1165,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C29">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -1179,16 +1182,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
@@ -1196,19 +1199,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C31">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -1216,16 +1219,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -1233,16 +1236,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -1250,16 +1253,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
@@ -1267,19 +1270,19 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
@@ -1287,16 +1290,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C36">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F36" t="s">
         <v>10</v>
@@ -1304,16 +1307,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
@@ -1321,16 +1324,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C38">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
@@ -1338,19 +1341,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C39">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -1358,16 +1361,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C40">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
@@ -1375,16 +1378,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C41">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
@@ -1392,16 +1395,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D42" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F42" t="s">
         <v>10</v>
@@ -1409,19 +1412,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C43">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F43" t="s">
         <v>10</v>
@@ -1429,16 +1432,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C44">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F44" t="s">
         <v>10</v>
@@ -1446,16 +1449,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C45">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D45" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
@@ -1463,16 +1466,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C46">
         <v>262144</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F46" t="s">
         <v>10</v>
@@ -1480,19 +1483,19 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C47">
         <v>262144</v>
       </c>
       <c r="D47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F47" t="s">
         <v>10</v>
@@ -1500,16 +1503,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C48">
         <v>262144</v>
       </c>
       <c r="D48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F48" t="s">
         <v>10</v>
@@ -1517,16 +1520,16 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C49">
         <v>262144</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F49" t="s">
         <v>10</v>
@@ -1534,16 +1537,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C50">
         <v>262144</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
@@ -1551,19 +1554,19 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C51">
         <v>262144</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F51" t="s">
         <v>10</v>
@@ -1571,16 +1574,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>262144</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F52" t="s">
         <v>10</v>
@@ -1588,16 +1591,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C53">
         <v>262144</v>
       </c>
       <c r="D53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
@@ -1605,16 +1608,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F54" t="s">
         <v>10</v>
@@ -1622,19 +1625,19 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C55">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E55" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F55" t="s">
         <v>10</v>
@@ -1642,16 +1645,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F56" t="s">
         <v>10</v>
@@ -1659,16 +1662,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C57">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F57" t="s">
         <v>10</v>
@@ -1676,16 +1679,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F58" t="s">
         <v>10</v>
@@ -1693,19 +1696,19 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E59" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F59" t="s">
         <v>10</v>
@@ -1713,16 +1716,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C60">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D60" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F60" t="s">
         <v>10</v>
@@ -1730,16 +1733,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
@@ -1747,16 +1750,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>262144</v>
       </c>
       <c r="D62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F62" t="s">
         <v>10</v>
@@ -1764,19 +1767,19 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C63">
         <v>262144</v>
       </c>
       <c r="D63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E63" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F63" t="s">
         <v>10</v>
@@ -1784,16 +1787,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C64">
         <v>262144</v>
       </c>
       <c r="D64" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F64" t="s">
         <v>10</v>
@@ -1801,16 +1804,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B65" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C65">
         <v>262144</v>
       </c>
       <c r="D65" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F65" t="s">
         <v>10</v>
@@ -1818,16 +1821,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C66">
         <v>262144</v>
       </c>
       <c r="D66" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F66" t="s">
         <v>10</v>
@@ -1835,19 +1838,19 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C67">
         <v>262144</v>
       </c>
       <c r="D67" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E67" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F67" t="s">
         <v>10</v>
@@ -1855,16 +1858,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C68">
         <v>262144</v>
       </c>
       <c r="D68" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F68" t="s">
         <v>10</v>
@@ -1872,16 +1875,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C69">
         <v>262144</v>
       </c>
       <c r="D69" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F69" t="s">
         <v>10</v>
@@ -1889,16 +1892,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B70" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C70">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D70" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F70" t="s">
         <v>10</v>
@@ -1906,19 +1909,19 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C71">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E71" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
         <v>10</v>
@@ -1926,16 +1929,16 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C72">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F72" t="s">
         <v>10</v>
@@ -1943,16 +1946,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B73" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C73">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D73" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F73" t="s">
         <v>10</v>
@@ -1960,16 +1963,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C74">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D74" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F74" t="s">
         <v>10</v>
@@ -1977,19 +1980,19 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C75">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D75" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E75" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F75" t="s">
         <v>10</v>
@@ -1997,16 +2000,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B76" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C76">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D76" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F76" t="s">
         <v>10</v>
@@ -2014,16 +2017,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B77" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C77">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D77" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F77" t="s">
         <v>10</v>
@@ -2031,16 +2034,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C78">
         <v>262144</v>
       </c>
       <c r="D78" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -2048,19 +2051,19 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C79">
         <v>262144</v>
       </c>
       <c r="D79" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -2068,16 +2071,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C80">
         <v>262144</v>
       </c>
       <c r="D80" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F80" t="s">
         <v>10</v>
@@ -2085,16 +2088,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B81" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C81">
         <v>262144</v>
       </c>
       <c r="D81" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F81" t="s">
         <v>10</v>
@@ -2102,16 +2105,16 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C82">
         <v>262144</v>
       </c>
       <c r="D82" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F82" t="s">
         <v>10</v>
@@ -2119,19 +2122,19 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B83" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C83">
         <v>262144</v>
       </c>
       <c r="D83" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E83" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -2139,16 +2142,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C84">
         <v>262144</v>
       </c>
       <c r="D84" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -2156,16 +2159,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C85">
         <v>262144</v>
       </c>
       <c r="D85" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
@@ -2173,16 +2176,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B86" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C86">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D86" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F86" t="s">
         <v>10</v>
@@ -2190,19 +2193,19 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C87">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D87" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E87" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F87" t="s">
         <v>10</v>
@@ -2210,16 +2213,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C88">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D88" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F88" t="s">
         <v>10</v>
@@ -2227,16 +2230,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C89">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D89" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -2244,16 +2247,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C90">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D90" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
@@ -2261,19 +2264,19 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B91" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D91" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E91" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -2281,16 +2284,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B92" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D92" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
@@ -2298,16 +2301,16 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B93" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C93">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D93" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F93" t="s">
         <v>10</v>
@@ -2315,16 +2318,16 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B94" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C94">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D94" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -2332,19 +2335,19 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B95" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C95">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D95" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E95" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F95" t="s">
         <v>10</v>
@@ -2352,16 +2355,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C96">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D96" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -2369,16 +2372,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B97" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C97">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D97" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -2386,16 +2389,16 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B98" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C98">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D98" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -2403,19 +2406,19 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B99" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C99">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D99" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E99" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -2423,16 +2426,16 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B100" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C100">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D100" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F100" t="s">
         <v>10</v>
@@ -2440,16 +2443,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B101" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C101">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D101" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F101" t="s">
         <v>10</v>
@@ -2457,16 +2460,16 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B102" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C102">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D102" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F102" t="s">
         <v>10</v>
@@ -2474,19 +2477,19 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B103" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C103">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D103" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E103" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F103" t="s">
         <v>10</v>
@@ -2494,16 +2497,16 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C104">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D104" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -2511,16 +2514,16 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B105" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C105">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D105" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -2528,16 +2531,16 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B106" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C106">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D106" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -2545,19 +2548,19 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B107" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C107">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D107" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E107" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F107" t="s">
         <v>10</v>
@@ -2565,16 +2568,16 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B108" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C108">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D108" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -2582,16 +2585,16 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B109" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C109">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F109" t="s">
         <v>10</v>
@@ -2599,158 +2602,158 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B110" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C110">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D110" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F110" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B111" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C111">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D111" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E111" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F111" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B112" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C112">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D112" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F112" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B113" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C113">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D113" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F113" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B114" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C114">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D114" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F114" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C115">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D115" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E115" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F115" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B116" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C116">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D116" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F116" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B117" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C117">
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="D117" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F117" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C118">
         <v>262144</v>
       </c>
       <c r="D118" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
@@ -2758,19 +2761,19 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C119">
         <v>262144</v>
       </c>
       <c r="D119" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E119" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -2778,16 +2781,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C120">
         <v>262144</v>
       </c>
       <c r="D120" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F120" t="s">
         <v>10</v>
@@ -2795,16 +2798,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C121">
         <v>262144</v>
       </c>
       <c r="D121" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F121" t="s">
         <v>10</v>
@@ -2812,16 +2815,16 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C122">
         <v>262144</v>
       </c>
       <c r="D122" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F122" t="s">
         <v>10</v>
@@ -2829,19 +2832,19 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C123">
         <v>262144</v>
       </c>
       <c r="D123" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E123" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F123" t="s">
         <v>10</v>
@@ -2849,16 +2852,16 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C124">
         <v>262144</v>
       </c>
       <c r="D124" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F124" t="s">
         <v>10</v>
@@ -2866,16 +2869,16 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C125">
         <v>262144</v>
       </c>
       <c r="D125" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F125" t="s">
         <v>10</v>
@@ -2883,16 +2886,16 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B126" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C126">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D126" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F126" t="s">
         <v>10</v>
@@ -2900,19 +2903,19 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B127" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C127">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D127" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E127" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F127" t="s">
         <v>10</v>
@@ -2920,16 +2923,16 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B128" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C128">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D128" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -2937,16 +2940,16 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B129" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C129">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D129" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F129" t="s">
         <v>10</v>
@@ -2954,16 +2957,16 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B130" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D130" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F130" t="s">
         <v>10</v>
@@ -2971,19 +2974,19 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B131" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C131">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D131" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E131" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -2991,16 +2994,16 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B132" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C132">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D132" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -3008,16 +3011,16 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B133" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C133">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D133" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
@@ -3025,16 +3028,16 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B134" t="s">
         <v>8</v>
       </c>
       <c r="C134">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D134" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -3042,19 +3045,19 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B135" t="s">
         <v>8</v>
       </c>
       <c r="C135">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D135" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E135" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -3062,16 +3065,16 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B136" t="s">
         <v>8</v>
       </c>
       <c r="C136">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D136" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F136" t="s">
         <v>10</v>
@@ -3079,16 +3082,16 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B137" t="s">
         <v>8</v>
       </c>
       <c r="C137">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D137" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F137" t="s">
         <v>10</v>
@@ -3096,16 +3099,16 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
       </c>
       <c r="C138">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D138" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F138" t="s">
         <v>10</v>
@@ -3113,19 +3116,19 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
       </c>
       <c r="C139">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D139" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E139" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F139" t="s">
         <v>10</v>
@@ -3133,16 +3136,16 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
       </c>
       <c r="C140">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D140" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F140" t="s">
         <v>10</v>
@@ -3150,16 +3153,16 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B141" t="s">
         <v>8</v>
       </c>
       <c r="C141">
-        <v>32768</v>
+        <v>16384</v>
       </c>
       <c r="D141" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F141" t="s">
         <v>10</v>
@@ -3167,16 +3170,16 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B142" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D142" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F142" t="s">
         <v>10</v>
@@ -3184,19 +3187,19 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B143" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C143">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D143" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E143" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F143" t="s">
         <v>10</v>
@@ -3204,16 +3207,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B144" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D144" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F144" t="s">
         <v>10</v>
@@ -3221,16 +3224,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B145" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C145">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D145" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
@@ -3238,16 +3241,16 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B146" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C146">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D146" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -3255,19 +3258,19 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B147" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C147">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D147" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E147" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F147" t="s">
         <v>10</v>
@@ -3275,16 +3278,16 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B148" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C148">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D148" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F148" t="s">
         <v>10</v>
@@ -3292,16 +3295,16 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B149" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C149">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D149" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F149" t="s">
         <v>10</v>
@@ -3309,16 +3312,16 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B150" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C150">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D150" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F150" t="s">
         <v>10</v>
@@ -3326,19 +3329,19 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B151" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C151">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D151" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E151" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -3346,16 +3349,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B152" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C152">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D152" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
@@ -3363,16 +3366,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B153" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C153">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D153" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F153" t="s">
         <v>10</v>
@@ -3380,16 +3383,16 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B154" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C154">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D154" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F154" t="s">
         <v>10</v>
@@ -3397,19 +3400,19 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B155" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C155">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D155" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E155" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F155" t="s">
         <v>10</v>
@@ -3417,16 +3420,16 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B156" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C156">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D156" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F156" t="s">
         <v>10</v>
@@ -3434,16 +3437,16 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B157" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="C157">
-        <v>131072</v>
+        <v>16384</v>
       </c>
       <c r="D157" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F157" t="s">
         <v>10</v>
@@ -3451,16 +3454,16 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
       </c>
       <c r="C158">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D158" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F158" t="s">
         <v>10</v>
@@ -3468,19 +3471,19 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
       </c>
       <c r="C159">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D159" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E159" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F159" t="s">
         <v>10</v>
@@ -3488,16 +3491,16 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
       </c>
       <c r="C160">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D160" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F160" t="s">
         <v>10</v>
@@ -3505,16 +3508,16 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
       </c>
       <c r="C161">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D161" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F161" t="s">
         <v>10</v>
@@ -3522,16 +3525,16 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
       </c>
       <c r="C162">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D162" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F162" t="s">
         <v>10</v>
@@ -3539,19 +3542,19 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
       </c>
       <c r="C163">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D163" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E163" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
@@ -3559,16 +3562,16 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
       </c>
       <c r="C164">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D164" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F164" t="s">
         <v>10</v>
@@ -3576,16 +3579,16 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
       </c>
       <c r="C165">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D165" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -3593,16 +3596,16 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B166" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C166">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D166" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
@@ -3610,19 +3613,19 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B167" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C167">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D167" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E167" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -3630,16 +3633,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B168" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C168">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D168" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F168" t="s">
         <v>10</v>
@@ -3647,16 +3650,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B169" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C169">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D169" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -3664,16 +3667,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B170" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C170">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D170" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F170" t="s">
         <v>10</v>
@@ -3681,19 +3684,19 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B171" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C171">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D171" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E171" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F171" t="s">
         <v>10</v>
@@ -3701,16 +3704,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B172" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C172">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D172" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F172" t="s">
         <v>10</v>
@@ -3718,16 +3721,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B173" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C173">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D173" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -3735,16 +3738,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C174">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D174" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F174" t="s">
         <v>10</v>
@@ -3752,19 +3755,19 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B175" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C175">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D175" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E175" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F175" t="s">
         <v>10</v>
@@ -3772,16 +3775,16 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B176" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C176">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D176" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -3789,16 +3792,16 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B177" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C177">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D177" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F177" t="s">
         <v>10</v>
@@ -3806,16 +3809,16 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B178" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C178">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D178" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
@@ -3823,19 +3826,19 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B179" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C179">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D179" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E179" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -3843,16 +3846,16 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B180" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C180">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D180" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F180" t="s">
         <v>10</v>
@@ -3860,16 +3863,16 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B181" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C181">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D181" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
tested 3 times.. and improved
</commit_message>
<xml_diff>
--- a/roundtable.xlsx
+++ b/roundtable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="124">
   <si>
     <t>Synergy Roundtable</t>
   </si>
@@ -37,25 +37,154 @@
     <t>Status</t>
   </si>
   <si>
+    <t>CTC Synergy HE21, bay 10</t>
+  </si>
+  <si>
+    <t>Synergy 480 Gen9</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:50</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:59</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:04:58</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:5b</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 1</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:70</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:51</t>
+  </si>
+  <si>
+    <t>94:57:A5:08:F5:78</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:53</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 4</t>
+  </si>
+  <si>
+    <t>Synergy 480 Gen10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:20</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:41</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:45:28</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:43</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE21, bay 5</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen10</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:10</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:11</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:18</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:19</t>
+  </si>
+  <si>
     <t>CTC Synergy HE01, bay 1</t>
   </si>
   <si>
-    <t>Synergy 480 Gen10</t>
-  </si>
-  <si>
     <t>94:F1:28:96:63:F0</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:59</t>
+    <t>10:00:26:1d:1a:80:00:15</t>
   </si>
   <si>
     <t>94:F1:28:96:63:F8</t>
   </si>
   <si>
-    <t>10:00:42:db:36:d0:00:5b</t>
+    <t>10:00:26:1d:1a:80:00:17</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 2</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:5B:00</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:E1:5B:01</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:5B:08</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:E1:5B:09</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 9</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:65:80</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:65:81</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:65:88</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:65:89</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 8</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:63:A0</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:63:A1</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:63:A8</t>
+  </si>
+  <si>
+    <t>10:00:94:F1:28:96:63:A9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 3</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:99:00</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:65</t>
+  </si>
+  <si>
+    <t>9C:DC:71:E1:99:08</t>
+  </si>
+  <si>
+    <t>10:00:26:1d:1a:80:00:67</t>
   </si>
   <si>
     <t>CTC Synergy HE01, bay 7</t>
@@ -64,24 +193,51 @@
     <t>9C:DC:71:E1:63:70</t>
   </si>
   <si>
-    <t>Warning</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:63:71</t>
+    <t>10:00:26:1d:1a:80:00:61</t>
   </si>
   <si>
     <t>9C:DC:71:E1:63:78</t>
   </si>
   <si>
-    <t>10:00:9C:DC:71:E1:63:79</t>
+    <t>10:00:26:1d:1a:80:00:63</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 4</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:60</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:61</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:68</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:69</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 2</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:90</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:91</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:02:98</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:02:99</t>
   </si>
   <si>
     <t>CTC Synergy HE11, bay 5</t>
   </si>
   <si>
-    <t>Synergy 480 Gen9</t>
-  </si>
-  <si>
     <t>94:18:82:39:21:F0</t>
   </si>
   <si>
@@ -94,6 +250,81 @@
     <t>10:00:94:18:82:39:21:F9</t>
   </si>
   <si>
+    <t>CTC Synergy HE11, bay 6</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:10</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:11</t>
+  </si>
+  <si>
+    <t>94:18:82:39:BC:18</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:BC:19</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 9</t>
+  </si>
+  <si>
+    <t>94:18:82:39:9B:60</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:9B:61</t>
+  </si>
+  <si>
+    <t>94:18:82:39:9B:68</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:9B:69</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 3</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:00:50</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:00:51</t>
+  </si>
+  <si>
+    <t>9C:DC:71:9D:00:58</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:9D:00:59</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 7</t>
+  </si>
+  <si>
+    <t>94:18:82:39:E3:E0</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:E3:E1</t>
+  </si>
+  <si>
+    <t>94:18:82:39:E3:E8</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:E3:E9</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE11, bay 8</t>
+  </si>
+  <si>
+    <t>94:18:82:39:68:20</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:68:21</t>
+  </si>
+  <si>
+    <t>94:18:82:39:68:28</t>
+  </si>
+  <si>
+    <t>10:00:94:18:82:39:68:29</t>
+  </si>
+  <si>
     <t>CTC Synergy HE11, bay 10</t>
   </si>
   <si>
@@ -109,34 +340,22 @@
     <t>10:00:9C:DC:71:9D:04:79</t>
   </si>
   <si>
-    <t>CTC Synergy HE11, bay 9</t>
-  </si>
-  <si>
-    <t>94:18:82:39:9B:60</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:9B:61</t>
-  </si>
-  <si>
-    <t>94:18:82:39:9B:68</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:9B:69</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 2</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:90</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:91</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:98</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:99</t>
+    <t>CTC Synergy HE21, bay 6</t>
+  </si>
+  <si>
+    <t>Synergy 660 Gen9</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C0</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C1</t>
+  </si>
+  <si>
+    <t>14:02:EC:C8:53:C8</t>
+  </si>
+  <si>
+    <t>10:00:14:02:EC:C8:53:C9</t>
   </si>
   <si>
     <t>CTC Synergy HE21, bay 2</t>
@@ -145,58 +364,13 @@
     <t>14:02:EC:C8:32:50</t>
   </si>
   <si>
-    <t>10:00:42:db:36:d0:00:91</t>
+    <t>10:00:26:1d:1a:80:00:55</t>
   </si>
   <si>
     <t>14:02:EC:C8:32:58</t>
   </si>
   <si>
-    <t>10:00:42:db:36:d0:00:93</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 6</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:10</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:11</t>
-  </si>
-  <si>
-    <t>94:18:82:39:BC:18</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:BC:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 1</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:70</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8d</t>
-  </si>
-  <si>
-    <t>94:57:A5:08:F5:78</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:00:8f</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:50</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:02:0b</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:04:58</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:02:0d</t>
+    <t>10:00:26:1d:1a:80:00:57</t>
   </si>
   <si>
     <t>CTC Synergy HE21, bay 3</t>
@@ -205,184 +379,13 @@
     <t>9C:DC:71:DF:4B:A0</t>
   </si>
   <si>
-    <t>10:00:42:db:36:d0:01:d1</t>
+    <t>10:00:9C:DC:71:DF:4B:A1</t>
   </si>
   <si>
     <t>9C:DC:71:DF:4B:A8</t>
   </si>
   <si>
-    <t>10:00:42:db:36:d0:01:d3</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 5</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen10</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:10</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:11</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:18</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 4</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:20</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:45:21</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:45:28</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:45:29</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE21, bay 6</t>
-  </si>
-  <si>
-    <t>Synergy 660 Gen9</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C0</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C1</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:53:C8</t>
-  </si>
-  <si>
-    <t>10:00:14:02:EC:C8:53:C9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 8</t>
-  </si>
-  <si>
-    <t>94:18:82:39:68:20</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:68:21</t>
-  </si>
-  <si>
-    <t>94:18:82:39:68:28</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:68:29</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 7</t>
-  </si>
-  <si>
-    <t>94:18:82:39:E3:E0</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:E3:E1</t>
-  </si>
-  <si>
-    <t>94:18:82:39:E3:E8</t>
-  </si>
-  <si>
-    <t>10:00:94:18:82:39:E3:E9</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 2</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:5B:00</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:5B:01</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:5B:08</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:5B:09</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 3</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:99:00</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:99:01</t>
-  </si>
-  <si>
-    <t>9C:DC:71:E1:99:08</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:E1:99:09</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 8</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:63:A0</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:01:c5</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:63:A8</t>
-  </si>
-  <si>
-    <t>10:00:42:db:36:d0:01:c7</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 9</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:65:80</t>
-  </si>
-  <si>
-    <t>10:00:94:F1:28:96:65:81</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:65:88</t>
-  </si>
-  <si>
-    <t>10:00:94:F1:28:96:65:89</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 4</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:60</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:61</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:02:68</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:02:69</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE11, bay 3</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:00:50</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:00:51</t>
-  </si>
-  <si>
-    <t>9C:DC:71:9D:00:58</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:9D:00:59</t>
+    <t>10:00:9C:DC:71:DF:4B:A9</t>
   </si>
 </sst>
 </file>
@@ -762,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -779,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -799,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -816,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -833,7 +836,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -850,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -870,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -887,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -904,13 +907,13 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -921,16 +924,16 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -941,13 +944,13 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -958,13 +961,13 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -975,13 +978,13 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -992,16 +995,16 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" t="s">
-        <v>19</v>
-      </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1012,13 +1015,13 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1029,27 +1032,27 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>16384</v>
+        <v>65536</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>65536</v>
+      </c>
+      <c r="D22" t="s">
         <v>21</v>
-      </c>
-      <c r="C22">
-        <v>262144</v>
-      </c>
-      <c r="D22" t="s">
-        <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
@@ -1057,19 +1060,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>65536</v>
+      </c>
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>262144</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>23</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -1077,16 +1080,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>65536</v>
+      </c>
+      <c r="D24" t="s">
         <v>21</v>
-      </c>
-      <c r="C24">
-        <v>262144</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
@@ -1094,16 +1097,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>65536</v>
+      </c>
+      <c r="D25" t="s">
         <v>21</v>
-      </c>
-      <c r="C25">
-        <v>262144</v>
-      </c>
-      <c r="D25" t="s">
-        <v>22</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
@@ -1111,16 +1114,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -1128,19 +1131,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
         <v>24</v>
-      </c>
-      <c r="E27" t="s">
-        <v>25</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -1148,16 +1151,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
@@ -1165,16 +1168,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -1182,1152 +1185,1152 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
       <c r="C30">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
       <c r="C31">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
         <v>26</v>
       </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
       <c r="C32">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
       <c r="C33">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
         <v>26</v>
       </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
       <c r="C34">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
       <c r="C35">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
       <c r="C36">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
         <v>26</v>
       </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
       <c r="C37">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C44">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C46">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E55" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D56" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C57">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D57" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C59">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C62">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C63">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D63" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E63" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D64" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F64" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D65" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F65" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C66">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D66" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E67" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C68">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D68" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C69">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D69" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C70">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D70" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C71">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D71" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F71" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D73" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C74">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C75">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D75" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E75" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F75" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C76">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D76" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F76" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C77">
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="D77" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F77" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C78">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D78" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C79">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D79" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F79" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D80" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F80" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D81" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D82" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C83">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D83" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E83" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D84" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C85">
-        <v>262144</v>
+        <v>16384</v>
       </c>
       <c r="D85" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
       <c r="C86">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D86" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
       <c r="C87">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D87" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E87" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
       </c>
       <c r="C88">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D88" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
       </c>
       <c r="C89">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D89" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F89" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="C90">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D90" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
       </c>
       <c r="C91">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D91" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E91" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
       <c r="C92">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D92" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
       </c>
       <c r="C93">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D93" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F93" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D94" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -2335,19 +2338,19 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B95" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C95">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D95" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E95" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F95" t="s">
         <v>10</v>
@@ -2355,16 +2358,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D96" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -2372,16 +2375,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B97" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C97">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D97" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -2389,16 +2392,16 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B98" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C98">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D98" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -2406,19 +2409,19 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B99" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C99">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D99" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E99" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -2426,16 +2429,16 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B100" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C100">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D100" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F100" t="s">
         <v>10</v>
@@ -2443,16 +2446,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B101" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="C101">
-        <v>32768</v>
+        <v>262144</v>
       </c>
       <c r="D101" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F101" t="s">
         <v>10</v>
@@ -2460,172 +2463,172 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
       </c>
       <c r="C102">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D102" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
       </c>
       <c r="C103">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D103" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E103" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F103" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
       </c>
       <c r="C104">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D104" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F104" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
       </c>
       <c r="C105">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D105" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F105" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B106" t="s">
         <v>8</v>
       </c>
       <c r="C106">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D106" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F106" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
       </c>
       <c r="C107">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D107" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E107" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F107" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
       </c>
       <c r="C108">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D108" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F108" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
       </c>
       <c r="C109">
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="D109" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F109" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B110" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C110">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D110" t="s">
         <v>79</v>
       </c>
       <c r="F110" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C111">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D111" t="s">
         <v>79</v>
@@ -2634,69 +2637,69 @@
         <v>80</v>
       </c>
       <c r="F111" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B112" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C112">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D112" t="s">
         <v>79</v>
       </c>
       <c r="F112" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B113" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C113">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D113" t="s">
         <v>79</v>
       </c>
       <c r="F113" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B114" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C114">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D114" t="s">
         <v>81</v>
       </c>
       <c r="F114" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B115" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C115">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D115" t="s">
         <v>81</v>
@@ -2705,41 +2708,41 @@
         <v>82</v>
       </c>
       <c r="F115" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B116" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C116">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D116" t="s">
         <v>81</v>
       </c>
       <c r="F116" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B117" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="C117">
-        <v>131072</v>
+        <v>262144</v>
       </c>
       <c r="D117" t="s">
         <v>81</v>
       </c>
       <c r="F117" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2747,7 +2750,7 @@
         <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C118">
         <v>262144</v>
@@ -2764,7 +2767,7 @@
         <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C119">
         <v>262144</v>
@@ -2784,7 +2787,7 @@
         <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C120">
         <v>262144</v>
@@ -2801,7 +2804,7 @@
         <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C121">
         <v>262144</v>
@@ -2818,7 +2821,7 @@
         <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C122">
         <v>262144</v>
@@ -2835,7 +2838,7 @@
         <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C123">
         <v>262144</v>
@@ -2855,7 +2858,7 @@
         <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C124">
         <v>262144</v>
@@ -2872,7 +2875,7 @@
         <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C125">
         <v>262144</v>
@@ -2889,7 +2892,7 @@
         <v>88</v>
       </c>
       <c r="B126" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C126">
         <v>262144</v>
@@ -2898,7 +2901,7 @@
         <v>89</v>
       </c>
       <c r="F126" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2906,7 +2909,7 @@
         <v>88</v>
       </c>
       <c r="B127" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C127">
         <v>262144</v>
@@ -2918,7 +2921,7 @@
         <v>90</v>
       </c>
       <c r="F127" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2926,7 +2929,7 @@
         <v>88</v>
       </c>
       <c r="B128" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C128">
         <v>262144</v>
@@ -2935,7 +2938,7 @@
         <v>89</v>
       </c>
       <c r="F128" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2943,7 +2946,7 @@
         <v>88</v>
       </c>
       <c r="B129" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C129">
         <v>262144</v>
@@ -2952,7 +2955,7 @@
         <v>89</v>
       </c>
       <c r="F129" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -2960,7 +2963,7 @@
         <v>88</v>
       </c>
       <c r="B130" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C130">
         <v>262144</v>
@@ -2969,7 +2972,7 @@
         <v>91</v>
       </c>
       <c r="F130" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -2977,7 +2980,7 @@
         <v>88</v>
       </c>
       <c r="B131" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C131">
         <v>262144</v>
@@ -2989,7 +2992,7 @@
         <v>92</v>
       </c>
       <c r="F131" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -2997,7 +3000,7 @@
         <v>88</v>
       </c>
       <c r="B132" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C132">
         <v>262144</v>
@@ -3006,7 +3009,7 @@
         <v>91</v>
       </c>
       <c r="F132" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3014,7 +3017,7 @@
         <v>88</v>
       </c>
       <c r="B133" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C133">
         <v>262144</v>
@@ -3023,7 +3026,7 @@
         <v>91</v>
       </c>
       <c r="F133" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3034,7 +3037,7 @@
         <v>8</v>
       </c>
       <c r="C134">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D134" t="s">
         <v>94</v>
@@ -3051,7 +3054,7 @@
         <v>8</v>
       </c>
       <c r="C135">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D135" t="s">
         <v>94</v>
@@ -3071,7 +3074,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D136" t="s">
         <v>94</v>
@@ -3088,7 +3091,7 @@
         <v>8</v>
       </c>
       <c r="C137">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D137" t="s">
         <v>94</v>
@@ -3105,7 +3108,7 @@
         <v>8</v>
       </c>
       <c r="C138">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D138" t="s">
         <v>96</v>
@@ -3122,7 +3125,7 @@
         <v>8</v>
       </c>
       <c r="C139">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D139" t="s">
         <v>96</v>
@@ -3142,7 +3145,7 @@
         <v>8</v>
       </c>
       <c r="C140">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D140" t="s">
         <v>96</v>
@@ -3159,7 +3162,7 @@
         <v>8</v>
       </c>
       <c r="C141">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D141" t="s">
         <v>96</v>
@@ -3176,7 +3179,7 @@
         <v>8</v>
       </c>
       <c r="C142">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D142" t="s">
         <v>99</v>
@@ -3193,7 +3196,7 @@
         <v>8</v>
       </c>
       <c r="C143">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D143" t="s">
         <v>99</v>
@@ -3213,7 +3216,7 @@
         <v>8</v>
       </c>
       <c r="C144">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D144" t="s">
         <v>99</v>
@@ -3230,7 +3233,7 @@
         <v>8</v>
       </c>
       <c r="C145">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D145" t="s">
         <v>99</v>
@@ -3247,7 +3250,7 @@
         <v>8</v>
       </c>
       <c r="C146">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D146" t="s">
         <v>101</v>
@@ -3264,7 +3267,7 @@
         <v>8</v>
       </c>
       <c r="C147">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D147" t="s">
         <v>101</v>
@@ -3284,7 +3287,7 @@
         <v>8</v>
       </c>
       <c r="C148">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D148" t="s">
         <v>101</v>
@@ -3301,7 +3304,7 @@
         <v>8</v>
       </c>
       <c r="C149">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D149" t="s">
         <v>101</v>
@@ -3318,7 +3321,7 @@
         <v>8</v>
       </c>
       <c r="C150">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D150" t="s">
         <v>104</v>
@@ -3335,7 +3338,7 @@
         <v>8</v>
       </c>
       <c r="C151">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D151" t="s">
         <v>104</v>
@@ -3355,7 +3358,7 @@
         <v>8</v>
       </c>
       <c r="C152">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D152" t="s">
         <v>104</v>
@@ -3372,7 +3375,7 @@
         <v>8</v>
       </c>
       <c r="C153">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D153" t="s">
         <v>104</v>
@@ -3389,7 +3392,7 @@
         <v>8</v>
       </c>
       <c r="C154">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D154" t="s">
         <v>106</v>
@@ -3406,7 +3409,7 @@
         <v>8</v>
       </c>
       <c r="C155">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D155" t="s">
         <v>106</v>
@@ -3426,7 +3429,7 @@
         <v>8</v>
       </c>
       <c r="C156">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D156" t="s">
         <v>106</v>
@@ -3443,7 +3446,7 @@
         <v>8</v>
       </c>
       <c r="C157">
-        <v>16384</v>
+        <v>262144</v>
       </c>
       <c r="D157" t="s">
         <v>106</v>
@@ -3457,16 +3460,16 @@
         <v>108</v>
       </c>
       <c r="B158" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C158">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D158" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F158" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -3474,19 +3477,19 @@
         <v>108</v>
       </c>
       <c r="B159" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C159">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D159" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E159" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F159" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -3494,16 +3497,16 @@
         <v>108</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C160">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D160" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F160" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -3511,16 +3514,16 @@
         <v>108</v>
       </c>
       <c r="B161" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C161">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D161" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F161" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -3528,16 +3531,16 @@
         <v>108</v>
       </c>
       <c r="B162" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C162">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D162" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F162" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -3545,19 +3548,19 @@
         <v>108</v>
       </c>
       <c r="B163" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C163">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D163" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E163" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F163" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -3565,16 +3568,16 @@
         <v>108</v>
       </c>
       <c r="B164" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C164">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D164" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F164" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -3582,30 +3585,30 @@
         <v>108</v>
       </c>
       <c r="B165" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C165">
-        <v>16384</v>
+        <v>131072</v>
       </c>
       <c r="D165" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F165" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B166" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C166">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D166" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
@@ -3613,19 +3616,19 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B167" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C167">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D167" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E167" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -3633,16 +3636,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B168" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D168" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F168" t="s">
         <v>10</v>
@@ -3650,16 +3653,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B169" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C169">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D169" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -3667,16 +3670,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B170" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C170">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D170" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F170" t="s">
         <v>10</v>
@@ -3684,19 +3687,19 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B171" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C171">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D171" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E171" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F171" t="s">
         <v>10</v>
@@ -3704,16 +3707,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B172" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C172">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D172" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F172" t="s">
         <v>10</v>
@@ -3721,16 +3724,16 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B173" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C173">
-        <v>262144</v>
+        <v>65536</v>
       </c>
       <c r="D173" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -3738,16 +3741,16 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B174" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C174">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D174" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F174" t="s">
         <v>10</v>
@@ -3755,19 +3758,19 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B175" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C175">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D175" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E175" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F175" t="s">
         <v>10</v>
@@ -3775,16 +3778,16 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B176" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C176">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D176" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -3792,16 +3795,16 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B177" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C177">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D177" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F177" t="s">
         <v>10</v>
@@ -3809,16 +3812,16 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B178" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C178">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D178" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
@@ -3826,19 +3829,19 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B179" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C179">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D179" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E179" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -3846,16 +3849,16 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B180" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C180">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D180" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F180" t="s">
         <v>10</v>
@@ -3863,16 +3866,16 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B181" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C181">
-        <v>262144</v>
+        <v>32768</v>
       </c>
       <c r="D181" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added quick install section
</commit_message>
<xml_diff>
--- a/roundtable.xlsx
+++ b/roundtable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="118">
   <si>
     <t>Synergy Roundtable</t>
   </si>
@@ -49,13 +49,13 @@
     <t>OK</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:59</t>
+    <t>10:00:26:1d:1a:80:00:35</t>
   </si>
   <si>
     <t>9C:DC:71:9D:04:58</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:5b</t>
+    <t>10:00:26:1d:1a:80:00:37</t>
   </si>
   <si>
     <t>CTC Synergy HE21, bay 1</t>
@@ -64,13 +64,13 @@
     <t>94:57:A5:08:F5:70</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:51</t>
+    <t>10:00:26:1d:1a:80:00:31</t>
   </si>
   <si>
     <t>94:57:A5:08:F5:78</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:53</t>
+    <t>10:00:26:1d:1a:80:00:33</t>
   </si>
   <si>
     <t>CTC Synergy HE21, bay 4</t>
@@ -82,13 +82,13 @@
     <t>9C:DC:71:DF:45:20</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:41</t>
+    <t>10:00:9C:DC:71:DF:45:21</t>
   </si>
   <si>
     <t>9C:DC:71:DF:45:28</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:43</t>
+    <t>10:00:9C:DC:71:DF:45:29</t>
   </si>
   <si>
     <t>CTC Synergy HE21, bay 5</t>
@@ -100,31 +100,31 @@
     <t>9C:DC:71:DF:41:10</t>
   </si>
   <si>
+    <t>10:00:9C:DC:71:DF:41:11</t>
+  </si>
+  <si>
+    <t>9C:DC:71:DF:41:18</t>
+  </si>
+  <si>
+    <t>10:00:9C:DC:71:DF:41:19</t>
+  </si>
+  <si>
+    <t>CTC Synergy HE01, bay 1</t>
+  </si>
+  <si>
+    <t>94:F1:28:96:63:F0</t>
+  </si>
+  <si>
     <t>Warning</t>
   </si>
   <si>
-    <t>10:00:9C:DC:71:DF:41:11</t>
-  </si>
-  <si>
-    <t>9C:DC:71:DF:41:18</t>
-  </si>
-  <si>
-    <t>10:00:9C:DC:71:DF:41:19</t>
-  </si>
-  <si>
-    <t>CTC Synergy HE01, bay 1</t>
-  </si>
-  <si>
-    <t>94:F1:28:96:63:F0</t>
-  </si>
-  <si>
-    <t>10:00:26:1d:1a:80:00:15</t>
+    <t>10:00:94:F1:28:96:63:F1</t>
   </si>
   <si>
     <t>94:F1:28:96:63:F8</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:17</t>
+    <t>10:00:94:F1:28:96:63:F9</t>
   </si>
   <si>
     <t>CTC Synergy HE01, bay 2</t>
@@ -178,13 +178,13 @@
     <t>9C:DC:71:E1:99:00</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:65</t>
+    <t>10:00:9C:DC:71:E1:99:01</t>
   </si>
   <si>
     <t>9C:DC:71:E1:99:08</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:67</t>
+    <t>10:00:9C:DC:71:E1:99:09</t>
   </si>
   <si>
     <t>CTC Synergy HE01, bay 7</t>
@@ -193,13 +193,13 @@
     <t>9C:DC:71:E1:63:70</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:61</t>
+    <t>10:00:9C:DC:71:E1:63:71</t>
   </si>
   <si>
     <t>9C:DC:71:E1:63:78</t>
   </si>
   <si>
-    <t>10:00:26:1d:1a:80:00:63</t>
+    <t>10:00:9C:DC:71:E1:63:79</t>
   </si>
   <si>
     <t>CTC Synergy HE11, bay 4</t>
@@ -208,9 +208,6 @@
     <t>9C:DC:71:9D:02:60</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
     <t>10:00:9C:DC:71:9D:02:61</t>
   </si>
   <si>
@@ -358,34 +355,19 @@
     <t>10:00:14:02:EC:C8:53:C9</t>
   </si>
   <si>
-    <t>CTC Synergy HE21, bay 2</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:50</t>
-  </si>
-  <si>
-    <t>10:00:26:1d:1a:80:00:55</t>
-  </si>
-  <si>
-    <t>14:02:EC:C8:32:58</t>
-  </si>
-  <si>
-    <t>10:00:26:1d:1a:80:00:57</t>
-  </si>
-  <si>
     <t>CTC Synergy HE21, bay 3</t>
   </si>
   <si>
     <t>9C:DC:71:DF:4B:A0</t>
   </si>
   <si>
-    <t>10:00:9C:DC:71:DF:4B:A1</t>
+    <t>10:00:26:1d:1a:80:00:f9</t>
   </si>
   <si>
     <t>9C:DC:71:DF:4B:A8</t>
   </si>
   <si>
-    <t>10:00:9C:DC:71:DF:4B:A9</t>
+    <t>10:00:26:1d:1a:80:00:fb</t>
   </si>
 </sst>
 </file>
@@ -726,7 +708,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1197,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1214,10 +1196,10 @@
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1234,7 +1216,7 @@
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1251,7 +1233,7 @@
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1265,10 +1247,10 @@
         <v>32768</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1282,13 +1264,13 @@
         <v>32768</v>
       </c>
       <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
         <v>30</v>
       </c>
-      <c r="E35" t="s">
-        <v>31</v>
-      </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1302,10 +1284,10 @@
         <v>32768</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1319,86 +1301,86 @@
         <v>32768</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>16384</v>
+      </c>
+      <c r="D38" t="s">
         <v>32</v>
       </c>
-      <c r="B38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38">
-        <v>16384</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="F38" t="s">
         <v>33</v>
-      </c>
-      <c r="F38" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>16384</v>
+      </c>
+      <c r="D39" t="s">
         <v>32</v>
-      </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39">
-        <v>16384</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>16384</v>
+      </c>
+      <c r="D40" t="s">
         <v>32</v>
       </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40">
-        <v>16384</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
         <v>33</v>
-      </c>
-      <c r="F40" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>16384</v>
+      </c>
+      <c r="D41" t="s">
         <v>32</v>
       </c>
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41">
-        <v>16384</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
         <v>33</v>
-      </c>
-      <c r="F41" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -1410,12 +1392,12 @@
         <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -1430,12 +1412,12 @@
         <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -1447,12 +1429,12 @@
         <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
@@ -1464,7 +1446,7 @@
         <v>35</v>
       </c>
       <c r="F45" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1481,7 +1463,7 @@
         <v>38</v>
       </c>
       <c r="F46" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1501,7 +1483,7 @@
         <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1518,7 +1500,7 @@
         <v>38</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1535,7 +1517,7 @@
         <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1552,7 +1534,7 @@
         <v>40</v>
       </c>
       <c r="F50" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1572,7 +1554,7 @@
         <v>41</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1589,7 +1571,7 @@
         <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1606,7 +1588,7 @@
         <v>40</v>
       </c>
       <c r="F53" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1623,7 +1605,7 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1643,7 +1625,7 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1660,7 +1642,7 @@
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1677,7 +1659,7 @@
         <v>43</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1694,7 +1676,7 @@
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1714,7 +1696,7 @@
         <v>46</v>
       </c>
       <c r="F59" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1731,7 +1713,7 @@
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1748,7 +1730,7 @@
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1765,7 +1747,7 @@
         <v>48</v>
       </c>
       <c r="F62" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1785,7 +1767,7 @@
         <v>49</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1802,7 +1784,7 @@
         <v>48</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1819,7 +1801,7 @@
         <v>48</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1836,7 +1818,7 @@
         <v>50</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1856,7 +1838,7 @@
         <v>51</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1873,7 +1855,7 @@
         <v>50</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1890,7 +1872,7 @@
         <v>50</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1907,7 +1889,7 @@
         <v>53</v>
       </c>
       <c r="F70" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1927,7 +1909,7 @@
         <v>54</v>
       </c>
       <c r="F71" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1944,7 +1926,7 @@
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1961,7 +1943,7 @@
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1978,7 +1960,7 @@
         <v>55</v>
       </c>
       <c r="F74" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1998,7 +1980,7 @@
         <v>56</v>
       </c>
       <c r="F75" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2015,7 +1997,7 @@
         <v>55</v>
       </c>
       <c r="F76" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2032,7 +2014,7 @@
         <v>55</v>
       </c>
       <c r="F77" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2049,7 +2031,7 @@
         <v>58</v>
       </c>
       <c r="F78" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2069,7 +2051,7 @@
         <v>59</v>
       </c>
       <c r="F79" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2086,7 +2068,7 @@
         <v>58</v>
       </c>
       <c r="F80" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2103,7 +2085,7 @@
         <v>58</v>
       </c>
       <c r="F81" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2120,7 +2102,7 @@
         <v>60</v>
       </c>
       <c r="F82" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2140,7 +2122,7 @@
         <v>61</v>
       </c>
       <c r="F83" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2157,7 +2139,7 @@
         <v>60</v>
       </c>
       <c r="F84" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2174,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="F85" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2191,7 +2173,7 @@
         <v>63</v>
       </c>
       <c r="F86" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2208,10 +2190,10 @@
         <v>63</v>
       </c>
       <c r="E87" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F87" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2228,7 +2210,7 @@
         <v>63</v>
       </c>
       <c r="F88" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2245,7 +2227,7 @@
         <v>63</v>
       </c>
       <c r="F89" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2259,10 +2241,10 @@
         <v>262144</v>
       </c>
       <c r="D90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F90" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2276,13 +2258,13 @@
         <v>262144</v>
       </c>
       <c r="D91" t="s">
+        <v>65</v>
+      </c>
+      <c r="E91" t="s">
         <v>66</v>
       </c>
-      <c r="E91" t="s">
-        <v>67</v>
-      </c>
       <c r="F91" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2296,10 +2278,10 @@
         <v>262144</v>
       </c>
       <c r="D92" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F92" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2313,24 +2295,24 @@
         <v>262144</v>
       </c>
       <c r="D93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F93" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>262144</v>
+      </c>
+      <c r="D94" t="s">
         <v>68</v>
-      </c>
-      <c r="B94" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94">
-        <v>262144</v>
-      </c>
-      <c r="D94" t="s">
-        <v>69</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -2338,19 +2320,19 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95">
+        <v>262144</v>
+      </c>
+      <c r="D95" t="s">
         <v>68</v>
       </c>
-      <c r="B95" t="s">
-        <v>8</v>
-      </c>
-      <c r="C95">
-        <v>262144</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>69</v>
-      </c>
-      <c r="E95" t="s">
-        <v>70</v>
       </c>
       <c r="F95" t="s">
         <v>10</v>
@@ -2358,16 +2340,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
+        <v>67</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <v>262144</v>
+      </c>
+      <c r="D96" t="s">
         <v>68</v>
-      </c>
-      <c r="B96" t="s">
-        <v>8</v>
-      </c>
-      <c r="C96">
-        <v>262144</v>
-      </c>
-      <c r="D96" t="s">
-        <v>69</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -2375,16 +2357,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97">
+        <v>262144</v>
+      </c>
+      <c r="D97" t="s">
         <v>68</v>
-      </c>
-      <c r="B97" t="s">
-        <v>8</v>
-      </c>
-      <c r="C97">
-        <v>262144</v>
-      </c>
-      <c r="D97" t="s">
-        <v>69</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -2392,7 +2374,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -2401,7 +2383,7 @@
         <v>262144</v>
       </c>
       <c r="D98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -2409,7 +2391,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
@@ -2418,10 +2400,10 @@
         <v>262144</v>
       </c>
       <c r="D99" t="s">
+        <v>70</v>
+      </c>
+      <c r="E99" t="s">
         <v>71</v>
-      </c>
-      <c r="E99" t="s">
-        <v>72</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -2429,7 +2411,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -2438,7 +2420,7 @@
         <v>262144</v>
       </c>
       <c r="D100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F100" t="s">
         <v>10</v>
@@ -2446,7 +2428,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
@@ -2455,7 +2437,7 @@
         <v>262144</v>
       </c>
       <c r="D101" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F101" t="s">
         <v>10</v>
@@ -2463,78 +2445,78 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
+        <v>72</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>262144</v>
+      </c>
+      <c r="D102" t="s">
         <v>73</v>
       </c>
-      <c r="B102" t="s">
-        <v>8</v>
-      </c>
-      <c r="C102">
-        <v>262144</v>
-      </c>
-      <c r="D102" t="s">
-        <v>74</v>
-      </c>
       <c r="F102" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
+        <v>72</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103">
+        <v>262144</v>
+      </c>
+      <c r="D103" t="s">
         <v>73</v>
       </c>
-      <c r="B103" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103">
-        <v>262144</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>74</v>
       </c>
-      <c r="E103" t="s">
-        <v>75</v>
-      </c>
       <c r="F103" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
+        <v>72</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104">
+        <v>262144</v>
+      </c>
+      <c r="D104" t="s">
         <v>73</v>
       </c>
-      <c r="B104" t="s">
-        <v>8</v>
-      </c>
-      <c r="C104">
-        <v>262144</v>
-      </c>
-      <c r="D104" t="s">
-        <v>74</v>
-      </c>
       <c r="F104" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
+        <v>72</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105">
+        <v>262144</v>
+      </c>
+      <c r="D105" t="s">
         <v>73</v>
       </c>
-      <c r="B105" t="s">
-        <v>8</v>
-      </c>
-      <c r="C105">
-        <v>262144</v>
-      </c>
-      <c r="D105" t="s">
-        <v>74</v>
-      </c>
       <c r="F105" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B106" t="s">
         <v>8</v>
@@ -2543,15 +2525,15 @@
         <v>262144</v>
       </c>
       <c r="D106" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F106" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
@@ -2560,18 +2542,18 @@
         <v>262144</v>
       </c>
       <c r="D107" t="s">
+        <v>75</v>
+      </c>
+      <c r="E107" t="s">
         <v>76</v>
       </c>
-      <c r="E107" t="s">
-        <v>77</v>
-      </c>
       <c r="F107" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -2580,15 +2562,15 @@
         <v>262144</v>
       </c>
       <c r="D108" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F108" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
@@ -2597,86 +2579,86 @@
         <v>262144</v>
       </c>
       <c r="D109" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F109" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>77</v>
+      </c>
+      <c r="B110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110">
+        <v>262144</v>
+      </c>
+      <c r="D110" t="s">
         <v>78</v>
       </c>
-      <c r="B110" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110">
-        <v>262144</v>
-      </c>
-      <c r="D110" t="s">
-        <v>79</v>
-      </c>
       <c r="F110" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
+        <v>77</v>
+      </c>
+      <c r="B111" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111">
+        <v>262144</v>
+      </c>
+      <c r="D111" t="s">
         <v>78</v>
       </c>
-      <c r="B111" t="s">
-        <v>8</v>
-      </c>
-      <c r="C111">
-        <v>262144</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>79</v>
       </c>
-      <c r="E111" t="s">
-        <v>80</v>
-      </c>
       <c r="F111" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
+        <v>77</v>
+      </c>
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112">
+        <v>262144</v>
+      </c>
+      <c r="D112" t="s">
         <v>78</v>
       </c>
-      <c r="B112" t="s">
-        <v>8</v>
-      </c>
-      <c r="C112">
-        <v>262144</v>
-      </c>
-      <c r="D112" t="s">
-        <v>79</v>
-      </c>
       <c r="F112" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
+        <v>77</v>
+      </c>
+      <c r="B113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113">
+        <v>262144</v>
+      </c>
+      <c r="D113" t="s">
         <v>78</v>
       </c>
-      <c r="B113" t="s">
-        <v>8</v>
-      </c>
-      <c r="C113">
-        <v>262144</v>
-      </c>
-      <c r="D113" t="s">
-        <v>79</v>
-      </c>
       <c r="F113" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B114" t="s">
         <v>8</v>
@@ -2685,15 +2667,15 @@
         <v>262144</v>
       </c>
       <c r="D114" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F114" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
@@ -2702,18 +2684,18 @@
         <v>262144</v>
       </c>
       <c r="D115" t="s">
+        <v>80</v>
+      </c>
+      <c r="E115" t="s">
         <v>81</v>
       </c>
-      <c r="E115" t="s">
-        <v>82</v>
-      </c>
       <c r="F115" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
@@ -2722,15 +2704,15 @@
         <v>262144</v>
       </c>
       <c r="D116" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F116" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
@@ -2739,24 +2721,24 @@
         <v>262144</v>
       </c>
       <c r="D117" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F117" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
+        <v>82</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118">
+        <v>262144</v>
+      </c>
+      <c r="D118" t="s">
         <v>83</v>
-      </c>
-      <c r="B118" t="s">
-        <v>8</v>
-      </c>
-      <c r="C118">
-        <v>262144</v>
-      </c>
-      <c r="D118" t="s">
-        <v>84</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
@@ -2764,19 +2746,19 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
+        <v>82</v>
+      </c>
+      <c r="B119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119">
+        <v>262144</v>
+      </c>
+      <c r="D119" t="s">
         <v>83</v>
       </c>
-      <c r="B119" t="s">
-        <v>8</v>
-      </c>
-      <c r="C119">
-        <v>262144</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
         <v>84</v>
-      </c>
-      <c r="E119" t="s">
-        <v>85</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -2784,16 +2766,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
+        <v>82</v>
+      </c>
+      <c r="B120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120">
+        <v>262144</v>
+      </c>
+      <c r="D120" t="s">
         <v>83</v>
-      </c>
-      <c r="B120" t="s">
-        <v>8</v>
-      </c>
-      <c r="C120">
-        <v>262144</v>
-      </c>
-      <c r="D120" t="s">
-        <v>84</v>
       </c>
       <c r="F120" t="s">
         <v>10</v>
@@ -2801,16 +2783,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
+        <v>82</v>
+      </c>
+      <c r="B121" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121">
+        <v>262144</v>
+      </c>
+      <c r="D121" t="s">
         <v>83</v>
-      </c>
-      <c r="B121" t="s">
-        <v>8</v>
-      </c>
-      <c r="C121">
-        <v>262144</v>
-      </c>
-      <c r="D121" t="s">
-        <v>84</v>
       </c>
       <c r="F121" t="s">
         <v>10</v>
@@ -2818,7 +2800,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
@@ -2827,7 +2809,7 @@
         <v>262144</v>
       </c>
       <c r="D122" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F122" t="s">
         <v>10</v>
@@ -2835,7 +2817,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
@@ -2844,10 +2826,10 @@
         <v>262144</v>
       </c>
       <c r="D123" t="s">
+        <v>85</v>
+      </c>
+      <c r="E123" t="s">
         <v>86</v>
-      </c>
-      <c r="E123" t="s">
-        <v>87</v>
       </c>
       <c r="F123" t="s">
         <v>10</v>
@@ -2855,7 +2837,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
@@ -2864,7 +2846,7 @@
         <v>262144</v>
       </c>
       <c r="D124" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F124" t="s">
         <v>10</v>
@@ -2872,7 +2854,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
@@ -2881,7 +2863,7 @@
         <v>262144</v>
       </c>
       <c r="D125" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F125" t="s">
         <v>10</v>
@@ -2889,78 +2871,78 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
+        <v>87</v>
+      </c>
+      <c r="B126" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126">
+        <v>262144</v>
+      </c>
+      <c r="D126" t="s">
         <v>88</v>
       </c>
-      <c r="B126" t="s">
-        <v>8</v>
-      </c>
-      <c r="C126">
-        <v>262144</v>
-      </c>
-      <c r="D126" t="s">
-        <v>89</v>
-      </c>
       <c r="F126" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
+        <v>87</v>
+      </c>
+      <c r="B127" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127">
+        <v>262144</v>
+      </c>
+      <c r="D127" t="s">
         <v>88</v>
       </c>
-      <c r="B127" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127">
-        <v>262144</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
         <v>89</v>
       </c>
-      <c r="E127" t="s">
-        <v>90</v>
-      </c>
       <c r="F127" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
+        <v>87</v>
+      </c>
+      <c r="B128" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128">
+        <v>262144</v>
+      </c>
+      <c r="D128" t="s">
         <v>88</v>
       </c>
-      <c r="B128" t="s">
-        <v>8</v>
-      </c>
-      <c r="C128">
-        <v>262144</v>
-      </c>
-      <c r="D128" t="s">
-        <v>89</v>
-      </c>
       <c r="F128" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
+        <v>87</v>
+      </c>
+      <c r="B129" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129">
+        <v>262144</v>
+      </c>
+      <c r="D129" t="s">
         <v>88</v>
       </c>
-      <c r="B129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129">
-        <v>262144</v>
-      </c>
-      <c r="D129" t="s">
-        <v>89</v>
-      </c>
       <c r="F129" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B130" t="s">
         <v>8</v>
@@ -2969,15 +2951,15 @@
         <v>262144</v>
       </c>
       <c r="D130" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F130" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B131" t="s">
         <v>8</v>
@@ -2986,18 +2968,18 @@
         <v>262144</v>
       </c>
       <c r="D131" t="s">
+        <v>90</v>
+      </c>
+      <c r="E131" t="s">
         <v>91</v>
       </c>
-      <c r="E131" t="s">
-        <v>92</v>
-      </c>
       <c r="F131" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B132" t="s">
         <v>8</v>
@@ -3006,15 +2988,15 @@
         <v>262144</v>
       </c>
       <c r="D132" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F132" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B133" t="s">
         <v>8</v>
@@ -3023,24 +3005,24 @@
         <v>262144</v>
       </c>
       <c r="D133" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F133" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
+        <v>92</v>
+      </c>
+      <c r="B134" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134">
+        <v>262144</v>
+      </c>
+      <c r="D134" t="s">
         <v>93</v>
-      </c>
-      <c r="B134" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134">
-        <v>262144</v>
-      </c>
-      <c r="D134" t="s">
-        <v>94</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -3048,19 +3030,19 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
+        <v>92</v>
+      </c>
+      <c r="B135" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135">
+        <v>262144</v>
+      </c>
+      <c r="D135" t="s">
         <v>93</v>
       </c>
-      <c r="B135" t="s">
-        <v>8</v>
-      </c>
-      <c r="C135">
-        <v>262144</v>
-      </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>94</v>
-      </c>
-      <c r="E135" t="s">
-        <v>95</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -3068,16 +3050,16 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
+        <v>92</v>
+      </c>
+      <c r="B136" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136">
+        <v>262144</v>
+      </c>
+      <c r="D136" t="s">
         <v>93</v>
-      </c>
-      <c r="B136" t="s">
-        <v>8</v>
-      </c>
-      <c r="C136">
-        <v>262144</v>
-      </c>
-      <c r="D136" t="s">
-        <v>94</v>
       </c>
       <c r="F136" t="s">
         <v>10</v>
@@ -3085,16 +3067,16 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
+        <v>92</v>
+      </c>
+      <c r="B137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137">
+        <v>262144</v>
+      </c>
+      <c r="D137" t="s">
         <v>93</v>
-      </c>
-      <c r="B137" t="s">
-        <v>8</v>
-      </c>
-      <c r="C137">
-        <v>262144</v>
-      </c>
-      <c r="D137" t="s">
-        <v>94</v>
       </c>
       <c r="F137" t="s">
         <v>10</v>
@@ -3102,7 +3084,7 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
@@ -3111,7 +3093,7 @@
         <v>262144</v>
       </c>
       <c r="D138" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F138" t="s">
         <v>10</v>
@@ -3119,7 +3101,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
@@ -3128,10 +3110,10 @@
         <v>262144</v>
       </c>
       <c r="D139" t="s">
+        <v>95</v>
+      </c>
+      <c r="E139" t="s">
         <v>96</v>
-      </c>
-      <c r="E139" t="s">
-        <v>97</v>
       </c>
       <c r="F139" t="s">
         <v>10</v>
@@ -3139,7 +3121,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
@@ -3148,7 +3130,7 @@
         <v>262144</v>
       </c>
       <c r="D140" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F140" t="s">
         <v>10</v>
@@ -3156,7 +3138,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B141" t="s">
         <v>8</v>
@@ -3165,7 +3147,7 @@
         <v>262144</v>
       </c>
       <c r="D141" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F141" t="s">
         <v>10</v>
@@ -3173,16 +3155,16 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
+        <v>97</v>
+      </c>
+      <c r="B142" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142">
+        <v>262144</v>
+      </c>
+      <c r="D142" t="s">
         <v>98</v>
-      </c>
-      <c r="B142" t="s">
-        <v>8</v>
-      </c>
-      <c r="C142">
-        <v>262144</v>
-      </c>
-      <c r="D142" t="s">
-        <v>99</v>
       </c>
       <c r="F142" t="s">
         <v>10</v>
@@ -3190,19 +3172,19 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
+        <v>97</v>
+      </c>
+      <c r="B143" t="s">
+        <v>8</v>
+      </c>
+      <c r="C143">
+        <v>262144</v>
+      </c>
+      <c r="D143" t="s">
         <v>98</v>
       </c>
-      <c r="B143" t="s">
-        <v>8</v>
-      </c>
-      <c r="C143">
-        <v>262144</v>
-      </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>99</v>
-      </c>
-      <c r="E143" t="s">
-        <v>100</v>
       </c>
       <c r="F143" t="s">
         <v>10</v>
@@ -3210,16 +3192,16 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
+        <v>97</v>
+      </c>
+      <c r="B144" t="s">
+        <v>8</v>
+      </c>
+      <c r="C144">
+        <v>262144</v>
+      </c>
+      <c r="D144" t="s">
         <v>98</v>
-      </c>
-      <c r="B144" t="s">
-        <v>8</v>
-      </c>
-      <c r="C144">
-        <v>262144</v>
-      </c>
-      <c r="D144" t="s">
-        <v>99</v>
       </c>
       <c r="F144" t="s">
         <v>10</v>
@@ -3227,16 +3209,16 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
+        <v>97</v>
+      </c>
+      <c r="B145" t="s">
+        <v>8</v>
+      </c>
+      <c r="C145">
+        <v>262144</v>
+      </c>
+      <c r="D145" t="s">
         <v>98</v>
-      </c>
-      <c r="B145" t="s">
-        <v>8</v>
-      </c>
-      <c r="C145">
-        <v>262144</v>
-      </c>
-      <c r="D145" t="s">
-        <v>99</v>
       </c>
       <c r="F145" t="s">
         <v>10</v>
@@ -3244,7 +3226,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B146" t="s">
         <v>8</v>
@@ -3253,7 +3235,7 @@
         <v>262144</v>
       </c>
       <c r="D146" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -3261,7 +3243,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
@@ -3270,10 +3252,10 @@
         <v>262144</v>
       </c>
       <c r="D147" t="s">
+        <v>100</v>
+      </c>
+      <c r="E147" t="s">
         <v>101</v>
-      </c>
-      <c r="E147" t="s">
-        <v>102</v>
       </c>
       <c r="F147" t="s">
         <v>10</v>
@@ -3281,7 +3263,7 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B148" t="s">
         <v>8</v>
@@ -3290,7 +3272,7 @@
         <v>262144</v>
       </c>
       <c r="D148" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F148" t="s">
         <v>10</v>
@@ -3298,7 +3280,7 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B149" t="s">
         <v>8</v>
@@ -3307,7 +3289,7 @@
         <v>262144</v>
       </c>
       <c r="D149" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F149" t="s">
         <v>10</v>
@@ -3315,16 +3297,16 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
+        <v>102</v>
+      </c>
+      <c r="B150" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150">
+        <v>262144</v>
+      </c>
+      <c r="D150" t="s">
         <v>103</v>
-      </c>
-      <c r="B150" t="s">
-        <v>8</v>
-      </c>
-      <c r="C150">
-        <v>262144</v>
-      </c>
-      <c r="D150" t="s">
-        <v>104</v>
       </c>
       <c r="F150" t="s">
         <v>10</v>
@@ -3332,19 +3314,19 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
+        <v>102</v>
+      </c>
+      <c r="B151" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151">
+        <v>262144</v>
+      </c>
+      <c r="D151" t="s">
         <v>103</v>
       </c>
-      <c r="B151" t="s">
-        <v>8</v>
-      </c>
-      <c r="C151">
-        <v>262144</v>
-      </c>
-      <c r="D151" t="s">
+      <c r="E151" t="s">
         <v>104</v>
-      </c>
-      <c r="E151" t="s">
-        <v>105</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -3352,16 +3334,16 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
+        <v>102</v>
+      </c>
+      <c r="B152" t="s">
+        <v>8</v>
+      </c>
+      <c r="C152">
+        <v>262144</v>
+      </c>
+      <c r="D152" t="s">
         <v>103</v>
-      </c>
-      <c r="B152" t="s">
-        <v>8</v>
-      </c>
-      <c r="C152">
-        <v>262144</v>
-      </c>
-      <c r="D152" t="s">
-        <v>104</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
@@ -3369,16 +3351,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
+        <v>102</v>
+      </c>
+      <c r="B153" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153">
+        <v>262144</v>
+      </c>
+      <c r="D153" t="s">
         <v>103</v>
-      </c>
-      <c r="B153" t="s">
-        <v>8</v>
-      </c>
-      <c r="C153">
-        <v>262144</v>
-      </c>
-      <c r="D153" t="s">
-        <v>104</v>
       </c>
       <c r="F153" t="s">
         <v>10</v>
@@ -3386,7 +3368,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B154" t="s">
         <v>8</v>
@@ -3395,7 +3377,7 @@
         <v>262144</v>
       </c>
       <c r="D154" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F154" t="s">
         <v>10</v>
@@ -3403,7 +3385,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
@@ -3412,10 +3394,10 @@
         <v>262144</v>
       </c>
       <c r="D155" t="s">
+        <v>105</v>
+      </c>
+      <c r="E155" t="s">
         <v>106</v>
-      </c>
-      <c r="E155" t="s">
-        <v>107</v>
       </c>
       <c r="F155" t="s">
         <v>10</v>
@@ -3423,7 +3405,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B156" t="s">
         <v>8</v>
@@ -3432,7 +3414,7 @@
         <v>262144</v>
       </c>
       <c r="D156" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F156" t="s">
         <v>10</v>
@@ -3440,7 +3422,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B157" t="s">
         <v>8</v>
@@ -3449,7 +3431,7 @@
         <v>262144</v>
       </c>
       <c r="D157" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F157" t="s">
         <v>10</v>
@@ -3457,158 +3439,158 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
+        <v>107</v>
+      </c>
+      <c r="B158" t="s">
         <v>108</v>
-      </c>
-      <c r="B158" t="s">
-        <v>109</v>
       </c>
       <c r="C158">
         <v>131072</v>
       </c>
       <c r="D158" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F158" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
+        <v>107</v>
+      </c>
+      <c r="B159" t="s">
         <v>108</v>
-      </c>
-      <c r="B159" t="s">
-        <v>109</v>
       </c>
       <c r="C159">
         <v>131072</v>
       </c>
       <c r="D159" t="s">
+        <v>109</v>
+      </c>
+      <c r="E159" t="s">
         <v>110</v>
       </c>
-      <c r="E159" t="s">
-        <v>111</v>
-      </c>
       <c r="F159" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
+        <v>107</v>
+      </c>
+      <c r="B160" t="s">
         <v>108</v>
-      </c>
-      <c r="B160" t="s">
-        <v>109</v>
       </c>
       <c r="C160">
         <v>131072</v>
       </c>
       <c r="D160" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F160" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
+        <v>107</v>
+      </c>
+      <c r="B161" t="s">
         <v>108</v>
-      </c>
-      <c r="B161" t="s">
-        <v>109</v>
       </c>
       <c r="C161">
         <v>131072</v>
       </c>
       <c r="D161" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F161" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
+        <v>107</v>
+      </c>
+      <c r="B162" t="s">
         <v>108</v>
-      </c>
-      <c r="B162" t="s">
-        <v>109</v>
       </c>
       <c r="C162">
         <v>131072</v>
       </c>
       <c r="D162" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F162" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
+        <v>107</v>
+      </c>
+      <c r="B163" t="s">
         <v>108</v>
-      </c>
-      <c r="B163" t="s">
-        <v>109</v>
       </c>
       <c r="C163">
         <v>131072</v>
       </c>
       <c r="D163" t="s">
+        <v>111</v>
+      </c>
+      <c r="E163" t="s">
         <v>112</v>
       </c>
-      <c r="E163" t="s">
-        <v>113</v>
-      </c>
       <c r="F163" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
+        <v>107</v>
+      </c>
+      <c r="B164" t="s">
         <v>108</v>
-      </c>
-      <c r="B164" t="s">
-        <v>109</v>
       </c>
       <c r="C164">
         <v>131072</v>
       </c>
       <c r="D164" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F164" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
+        <v>107</v>
+      </c>
+      <c r="B165" t="s">
         <v>108</v>
-      </c>
-      <c r="B165" t="s">
-        <v>109</v>
       </c>
       <c r="C165">
         <v>131072</v>
       </c>
       <c r="D165" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F165" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
+        <v>113</v>
+      </c>
+      <c r="B166" t="s">
+        <v>20</v>
+      </c>
+      <c r="C166">
+        <v>32768</v>
+      </c>
+      <c r="D166" t="s">
         <v>114</v>
-      </c>
-      <c r="B166" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166">
-        <v>65536</v>
-      </c>
-      <c r="D166" t="s">
-        <v>115</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
@@ -3616,19 +3598,19 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
+        <v>113</v>
+      </c>
+      <c r="B167" t="s">
+        <v>20</v>
+      </c>
+      <c r="C167">
+        <v>32768</v>
+      </c>
+      <c r="D167" t="s">
         <v>114</v>
       </c>
-      <c r="B167" t="s">
-        <v>8</v>
-      </c>
-      <c r="C167">
-        <v>65536</v>
-      </c>
-      <c r="D167" t="s">
+      <c r="E167" t="s">
         <v>115</v>
-      </c>
-      <c r="E167" t="s">
-        <v>116</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -3636,16 +3618,16 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
+        <v>113</v>
+      </c>
+      <c r="B168" t="s">
+        <v>20</v>
+      </c>
+      <c r="C168">
+        <v>32768</v>
+      </c>
+      <c r="D168" t="s">
         <v>114</v>
-      </c>
-      <c r="B168" t="s">
-        <v>8</v>
-      </c>
-      <c r="C168">
-        <v>65536</v>
-      </c>
-      <c r="D168" t="s">
-        <v>115</v>
       </c>
       <c r="F168" t="s">
         <v>10</v>
@@ -3653,16 +3635,16 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
+        <v>113</v>
+      </c>
+      <c r="B169" t="s">
+        <v>20</v>
+      </c>
+      <c r="C169">
+        <v>32768</v>
+      </c>
+      <c r="D169" t="s">
         <v>114</v>
-      </c>
-      <c r="B169" t="s">
-        <v>8</v>
-      </c>
-      <c r="C169">
-        <v>65536</v>
-      </c>
-      <c r="D169" t="s">
-        <v>115</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -3670,16 +3652,16 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B170" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C170">
-        <v>65536</v>
+        <v>32768</v>
       </c>
       <c r="D170" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F170" t="s">
         <v>10</v>
@@ -3687,19 +3669,19 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B171" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C171">
-        <v>65536</v>
+        <v>32768</v>
       </c>
       <c r="D171" t="s">
+        <v>116</v>
+      </c>
+      <c r="E171" t="s">
         <v>117</v>
-      </c>
-      <c r="E171" t="s">
-        <v>118</v>
       </c>
       <c r="F171" t="s">
         <v>10</v>
@@ -3707,16 +3689,16 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B172" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C172">
-        <v>65536</v>
+        <v>32768</v>
       </c>
       <c r="D172" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F172" t="s">
         <v>10</v>
@@ -3724,160 +3706,18 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C173">
-        <v>65536</v>
+        <v>32768</v>
       </c>
       <c r="D173" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F173" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6">
-      <c r="A174" t="s">
-        <v>119</v>
-      </c>
-      <c r="B174" t="s">
-        <v>20</v>
-      </c>
-      <c r="C174">
-        <v>32768</v>
-      </c>
-      <c r="D174" t="s">
-        <v>120</v>
-      </c>
-      <c r="F174" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6">
-      <c r="A175" t="s">
-        <v>119</v>
-      </c>
-      <c r="B175" t="s">
-        <v>20</v>
-      </c>
-      <c r="C175">
-        <v>32768</v>
-      </c>
-      <c r="D175" t="s">
-        <v>120</v>
-      </c>
-      <c r="E175" t="s">
-        <v>121</v>
-      </c>
-      <c r="F175" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
-      <c r="A176" t="s">
-        <v>119</v>
-      </c>
-      <c r="B176" t="s">
-        <v>20</v>
-      </c>
-      <c r="C176">
-        <v>32768</v>
-      </c>
-      <c r="D176" t="s">
-        <v>120</v>
-      </c>
-      <c r="F176" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
-      <c r="A177" t="s">
-        <v>119</v>
-      </c>
-      <c r="B177" t="s">
-        <v>20</v>
-      </c>
-      <c r="C177">
-        <v>32768</v>
-      </c>
-      <c r="D177" t="s">
-        <v>120</v>
-      </c>
-      <c r="F177" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
-      <c r="A178" t="s">
-        <v>119</v>
-      </c>
-      <c r="B178" t="s">
-        <v>20</v>
-      </c>
-      <c r="C178">
-        <v>32768</v>
-      </c>
-      <c r="D178" t="s">
-        <v>122</v>
-      </c>
-      <c r="F178" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
-      <c r="A179" t="s">
-        <v>119</v>
-      </c>
-      <c r="B179" t="s">
-        <v>20</v>
-      </c>
-      <c r="C179">
-        <v>32768</v>
-      </c>
-      <c r="D179" t="s">
-        <v>122</v>
-      </c>
-      <c r="E179" t="s">
-        <v>123</v>
-      </c>
-      <c r="F179" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="A180" t="s">
-        <v>119</v>
-      </c>
-      <c r="B180" t="s">
-        <v>20</v>
-      </c>
-      <c r="C180">
-        <v>32768</v>
-      </c>
-      <c r="D180" t="s">
-        <v>122</v>
-      </c>
-      <c r="F180" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
-      <c r="A181" t="s">
-        <v>119</v>
-      </c>
-      <c r="B181" t="s">
-        <v>20</v>
-      </c>
-      <c r="C181">
-        <v>32768</v>
-      </c>
-      <c r="D181" t="s">
-        <v>122</v>
-      </c>
-      <c r="F181" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>